<commit_message>
Lägger till Bolagsverket dokument-API: dokumentlista och hämta årsredovisningar
</commit_message>
<xml_diff>
--- a/Testdata API Vardefulla datamangder.xlsx
+++ b/Testdata API Vardefulla datamangder.xlsx
@@ -8,25 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnnikaRydén\OneDrive\ClientFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15769DBA-51B5-4E85-B707-50299D4B1A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C6B9A9-0A0F-4F01-B5A4-63A0A8689D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="6945" windowWidth="29040" windowHeight="15720" tabRatio="323" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="323" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ändringshistorik" sheetId="18" r:id="rId1"/>
     <sheet name="Resurs organisationer" sheetId="6" r:id="rId2"/>
-    <sheet name="Resurs dokumentlista" sheetId="19" r:id="rId3"/>
-    <sheet name="Övriga identitetsbeteckningar " sheetId="20" r:id="rId4"/>
+    <sheet name="Blad1" sheetId="21" r:id="rId3"/>
+    <sheet name="Blad2" sheetId="22" r:id="rId4"/>
+    <sheet name="Resurs dokumentlista" sheetId="19" r:id="rId5"/>
+    <sheet name="Övriga identitetsbeteckningar " sheetId="20" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_556003_8860">'Resurs organisationer'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="157">
   <si>
     <t>-</t>
   </si>
@@ -1122,6 +1137,33 @@
       </rPr>
       <t>Dataproducent: Bolagsverket eller SCB</t>
     </r>
+  </si>
+  <si>
+    <t>Datum </t>
+  </si>
+  <si>
+    <t>Transaktion </t>
+  </si>
+  <si>
+    <t>Belopp</t>
+  </si>
+  <si>
+    <t>Slutlig skatt</t>
+  </si>
+  <si>
+    <t>Avdragen skatt</t>
+  </si>
+  <si>
+    <t>Skattetillägg slutlig skatt</t>
+  </si>
+  <si>
+    <t>Preliminär skattereduktion för rot/rut/grön teknik</t>
+  </si>
+  <si>
+    <t>NYTT</t>
+  </si>
+  <si>
+    <t>SKILLNAD</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1557,22 +1599,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1601,24 +1661,7 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dålig" xfId="1" builtinId="27"/>
@@ -2035,11 +2078,11 @@
   </sheetPr>
   <dimension ref="A1:AA140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="A8:B8"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2078,14 +2121,14 @@
       <c r="F1" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="69" t="s">
+      <c r="H1" s="72"/>
+      <c r="I1" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="70"/>
+      <c r="J1" s="72"/>
       <c r="K1" s="13" t="s">
         <v>129</v>
       </c>
@@ -2115,14 +2158,14 @@
       <c r="F2" s="31">
         <v>198101032384</v>
       </c>
-      <c r="G2" s="79">
+      <c r="G2" s="85">
         <v>198101052382</v>
       </c>
-      <c r="H2" s="80"/>
-      <c r="I2" s="79">
+      <c r="H2" s="86"/>
+      <c r="I2" s="85">
         <v>193403223328</v>
       </c>
-      <c r="J2" s="80"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="52">
         <v>5567223705</v>
       </c>
@@ -2142,10 +2185,10 @@
       <c r="D3" s="54"/>
       <c r="E3" s="53"/>
       <c r="F3" s="55"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="56"/>
       <c r="L3" s="53"/>
       <c r="M3" s="53"/>
@@ -2169,14 +2212,14 @@
       <c r="F4" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="78"/>
-      <c r="I4" s="71" t="s">
+      <c r="H4" s="84"/>
+      <c r="I4" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="78"/>
+      <c r="J4" s="84"/>
       <c r="K4" s="42" t="s">
         <v>58</v>
       </c>
@@ -2247,14 +2290,14 @@
       <c r="F6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="67" t="s">
+      <c r="G6" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="71" t="s">
+      <c r="H6" s="74"/>
+      <c r="I6" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="72"/>
+      <c r="J6" s="78"/>
       <c r="K6" s="47" t="s">
         <v>16</v>
       </c>
@@ -2284,14 +2327,14 @@
       <c r="F7" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="71" t="s">
+      <c r="H7" s="74"/>
+      <c r="I7" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="72"/>
+      <c r="J7" s="78"/>
       <c r="K7" s="47" t="s">
         <v>54</v>
       </c>
@@ -2362,14 +2405,14 @@
       <c r="F9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="68"/>
-      <c r="I9" s="65" t="s">
+      <c r="H9" s="74"/>
+      <c r="I9" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="66"/>
+      <c r="J9" s="76"/>
       <c r="K9" s="32" t="s">
         <v>15</v>
       </c>
@@ -2399,10 +2442,10 @@
       <c r="F10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="67" t="s">
+      <c r="G10" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="68"/>
+      <c r="H10" s="74"/>
       <c r="I10" s="24">
         <v>42606</v>
       </c>
@@ -2438,10 +2481,10 @@
       <c r="F11" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="67" t="s">
+      <c r="G11" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="68"/>
+      <c r="H11" s="74"/>
       <c r="I11" s="38" t="s">
         <v>50</v>
       </c>
@@ -2477,14 +2520,14 @@
       <c r="F12" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="68"/>
-      <c r="I12" s="65" t="s">
+      <c r="H12" s="74"/>
+      <c r="I12" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="66"/>
+      <c r="J12" s="76"/>
       <c r="K12" s="32" t="s">
         <v>0</v>
       </c>
@@ -2514,10 +2557,10 @@
       <c r="F13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="83" t="s">
+      <c r="G13" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="84"/>
+      <c r="H13" s="68"/>
       <c r="I13" s="38" t="s">
         <v>37</v>
       </c>
@@ -2553,10 +2596,10 @@
       <c r="F14" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="83" t="s">
+      <c r="G14" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="84"/>
+      <c r="H14" s="68"/>
       <c r="I14" s="24" t="s">
         <v>39</v>
       </c>
@@ -2715,10 +2758,10 @@
       <c r="F18" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="81" t="s">
+      <c r="G18" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="82"/>
+      <c r="H18" s="66"/>
       <c r="I18" s="38" t="s">
         <v>4</v>
       </c>
@@ -2754,10 +2797,10 @@
       <c r="F19" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="81" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="82"/>
+      <c r="G19" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="66"/>
       <c r="I19" s="38" t="s">
         <v>11</v>
       </c>
@@ -2793,10 +2836,10 @@
       <c r="F20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="81" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="82"/>
+      <c r="G20" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="66"/>
       <c r="I20" s="38" t="s">
         <v>11</v>
       </c>
@@ -2820,7 +2863,7 @@
       <c r="A22" s="6"/>
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="85" t="s">
+      <c r="A23" s="69" t="s">
         <v>143</v>
       </c>
       <c r="B23" s="59" t="s">
@@ -2828,31 +2871,31 @@
       </c>
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="86"/>
+      <c r="A24" s="70"/>
       <c r="B24" s="59" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="86"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="59" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="86"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="59" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="86"/>
+      <c r="A27" s="70"/>
       <c r="B27" s="59" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="86"/>
+      <c r="A28" s="70"/>
       <c r="B28" s="59" t="s">
         <v>65</v>
       </c>
@@ -3328,17 +3371,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="24">
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="G9:H9"/>
@@ -3352,6 +3384,17 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="51" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -3359,6 +3402,284 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68152F34-4C61-41C5-9C39-A3BBEA315BEB}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="54.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="232" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="290" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="174" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="174" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="174" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFD399D-BAFD-477C-886D-7EDCF3226FF1}">
+  <dimension ref="F6:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H6" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F7" s="8">
+        <v>45363</v>
+      </c>
+      <c r="G7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="87">
+        <v>-56485</v>
+      </c>
+      <c r="I7">
+        <v>-36556</v>
+      </c>
+    </row>
+    <row r="8" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F8" s="8">
+        <v>45363</v>
+      </c>
+      <c r="G8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H8" s="87">
+        <v>65213</v>
+      </c>
+      <c r="I8">
+        <v>65213</v>
+      </c>
+    </row>
+    <row r="9" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F9" s="8">
+        <v>45363</v>
+      </c>
+      <c r="G9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H9" s="87">
+        <v>-10000</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F10" s="8"/>
+      <c r="H10" s="87">
+        <f>SUM(H7:H9)</f>
+        <v>-1272</v>
+      </c>
+      <c r="I10" s="87">
+        <f>SUM(I7:I9)</f>
+        <v>28657</v>
+      </c>
+      <c r="J10" s="87">
+        <f>I10-H10</f>
+        <v>29929</v>
+      </c>
+      <c r="K10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="J11" s="87"/>
+    </row>
+    <row r="12" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="J12" s="87"/>
+    </row>
+    <row r="13" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F13" s="8">
+        <v>45601</v>
+      </c>
+      <c r="G13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H13" s="87">
+        <v>-76131</v>
+      </c>
+      <c r="I13">
+        <v>-88398</v>
+      </c>
+      <c r="J13" s="87"/>
+    </row>
+    <row r="14" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F14" s="8">
+        <v>45601</v>
+      </c>
+      <c r="G14" t="s">
+        <v>152</v>
+      </c>
+      <c r="H14" s="87">
+        <v>95231</v>
+      </c>
+      <c r="I14">
+        <v>95231</v>
+      </c>
+      <c r="J14" s="87"/>
+    </row>
+    <row r="15" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F15" s="8">
+        <v>45601</v>
+      </c>
+      <c r="G15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="87">
+        <v>-3000</v>
+      </c>
+      <c r="J15" s="87"/>
+    </row>
+    <row r="16" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="H16" s="87">
+        <f>SUM(H13:H15)</f>
+        <v>16100</v>
+      </c>
+      <c r="I16" s="87">
+        <f>SUM(I13:I15)</f>
+        <v>6833</v>
+      </c>
+      <c r="J16" s="87">
+        <f t="shared" ref="J11:J16" si="0">I16-H16</f>
+        <v>-9267</v>
+      </c>
+      <c r="K16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="87"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="87"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="87"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F31" s="87"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3407,7 +3728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A51"/>
   <sheetViews>
@@ -3679,12 +4000,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Kommentar0 xmlns="055c4a11-8173-45d4-8412-20d21b900f07" xsi:nil="true"/>
+    <Kategori xmlns="055c4a11-8173-45d4-8412-20d21b900f07">Teknisk dokumentation</Kategori>
+    <M_x00e5_lgrupp xmlns="055c4a11-8173-45d4-8412-20d21b900f07">
+      <Value>Konsumenter</Value>
+      <Value>IT-leverantörer</Value>
+    </M_x00e5_lgrupp>
+    <Kommentar xmlns="055c4a11-8173-45d4-8412-20d21b900f07">OK</Kommentar>
+    <Syfte xmlns="055c4a11-8173-45d4-8412-20d21b900f07" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3870,24 +4197,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Kommentar0 xmlns="055c4a11-8173-45d4-8412-20d21b900f07" xsi:nil="true"/>
-    <Kategori xmlns="055c4a11-8173-45d4-8412-20d21b900f07">Teknisk dokumentation</Kategori>
-    <M_x00e5_lgrupp xmlns="055c4a11-8173-45d4-8412-20d21b900f07">
-      <Value>Konsumenter</Value>
-      <Value>IT-leverantörer</Value>
-    </M_x00e5_lgrupp>
-    <Kommentar xmlns="055c4a11-8173-45d4-8412-20d21b900f07">OK</Kommentar>
-    <Syfte xmlns="055c4a11-8173-45d4-8412-20d21b900f07" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{905DD5F0-F1C4-403B-AC12-3FD7F1CF9D2F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90CD9CF6-3488-4F16-8E76-7A648CC36ED2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="055c4a11-8173-45d4-8412-20d21b900f07"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3911,17 +4240,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90CD9CF6-3488-4F16-8E76-7A648CC36ED2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{905DD5F0-F1C4-403B-AC12-3FD7F1CF9D2F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="055c4a11-8173-45d4-8412-20d21b900f07"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Förbättrad datahantering från Bolagsverket API - lagt till detaljerad loggning och bättre fallback-värden
</commit_message>
<xml_diff>
--- a/Testdata API Vardefulla datamangder.xlsx
+++ b/Testdata API Vardefulla datamangder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnnikaRydén\OneDrive\ClientFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C6B9A9-0A0F-4F01-B5A4-63A0A8689D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35ECBF75-791F-4324-9488-1BA29B133F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="323" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="323" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ändringshistorik" sheetId="18" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="_556003_8860">'Resurs organisationer'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1170,7 +1171,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1235,8 +1236,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1276,6 +1292,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1419,11 +1440,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1599,40 +1621,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1661,9 +1686,27 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bra" xfId="2" builtinId="26"/>
     <cellStyle name="Dålig" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2082,7 +2125,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A20"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2102,7 +2145,7 @@
     <col min="14" max="27" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
@@ -2121,14 +2164,14 @@
       <c r="F1" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="72"/>
-      <c r="I1" s="71" t="s">
+      <c r="H1" s="77"/>
+      <c r="I1" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="72"/>
+      <c r="J1" s="77"/>
       <c r="K1" s="13" t="s">
         <v>129</v>
       </c>
@@ -2158,14 +2201,14 @@
       <c r="F2" s="31">
         <v>198101032384</v>
       </c>
-      <c r="G2" s="85">
+      <c r="G2" s="86">
         <v>198101052382</v>
       </c>
-      <c r="H2" s="86"/>
-      <c r="I2" s="85">
+      <c r="H2" s="87"/>
+      <c r="I2" s="86">
         <v>193403223328</v>
       </c>
-      <c r="J2" s="86"/>
+      <c r="J2" s="87"/>
       <c r="K2" s="52">
         <v>5567223705</v>
       </c>
@@ -2185,10 +2228,10 @@
       <c r="D3" s="54"/>
       <c r="E3" s="53"/>
       <c r="F3" s="55"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="82"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="56"/>
       <c r="L3" s="53"/>
       <c r="M3" s="53"/>
@@ -2212,14 +2255,14 @@
       <c r="F4" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="84"/>
-      <c r="I4" s="77" t="s">
+      <c r="H4" s="85"/>
+      <c r="I4" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="84"/>
+      <c r="J4" s="85"/>
       <c r="K4" s="42" t="s">
         <v>58</v>
       </c>
@@ -2290,14 +2333,14 @@
       <c r="F6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="74"/>
-      <c r="I6" s="77" t="s">
+      <c r="H6" s="75"/>
+      <c r="I6" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="78"/>
+      <c r="J6" s="79"/>
       <c r="K6" s="47" t="s">
         <v>16</v>
       </c>
@@ -2327,14 +2370,14 @@
       <c r="F7" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="74"/>
-      <c r="I7" s="77" t="s">
+      <c r="H7" s="75"/>
+      <c r="I7" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="78"/>
+      <c r="J7" s="79"/>
       <c r="K7" s="47" t="s">
         <v>54</v>
       </c>
@@ -2405,14 +2448,14 @@
       <c r="F9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="73" t="s">
+      <c r="G9" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="74"/>
-      <c r="I9" s="75" t="s">
+      <c r="H9" s="75"/>
+      <c r="I9" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="76"/>
+      <c r="J9" s="73"/>
       <c r="K9" s="32" t="s">
         <v>15</v>
       </c>
@@ -2442,10 +2485,10 @@
       <c r="F10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="73" t="s">
+      <c r="G10" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="74"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="24">
         <v>42606</v>
       </c>
@@ -2481,10 +2524,10 @@
       <c r="F11" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="73" t="s">
+      <c r="G11" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="74"/>
+      <c r="H11" s="75"/>
       <c r="I11" s="38" t="s">
         <v>50</v>
       </c>
@@ -2520,14 +2563,14 @@
       <c r="F12" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="73" t="s">
+      <c r="G12" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="74"/>
-      <c r="I12" s="75" t="s">
+      <c r="H12" s="75"/>
+      <c r="I12" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="76"/>
+      <c r="J12" s="73"/>
       <c r="K12" s="32" t="s">
         <v>0</v>
       </c>
@@ -2557,10 +2600,10 @@
       <c r="F13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="67" t="s">
+      <c r="G13" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="68"/>
+      <c r="H13" s="91"/>
       <c r="I13" s="38" t="s">
         <v>37</v>
       </c>
@@ -2596,10 +2639,10 @@
       <c r="F14" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="67" t="s">
+      <c r="G14" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="68"/>
+      <c r="H14" s="91"/>
       <c r="I14" s="24" t="s">
         <v>39</v>
       </c>
@@ -2758,10 +2801,10 @@
       <c r="F18" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="66"/>
+      <c r="H18" s="89"/>
       <c r="I18" s="38" t="s">
         <v>4</v>
       </c>
@@ -2797,10 +2840,10 @@
       <c r="F19" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="65" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="66"/>
+      <c r="G19" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="89"/>
       <c r="I19" s="38" t="s">
         <v>11</v>
       </c>
@@ -2836,10 +2879,10 @@
       <c r="F20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="65" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="66"/>
+      <c r="G20" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="89"/>
       <c r="I20" s="38" t="s">
         <v>11</v>
       </c>
@@ -2863,7 +2906,7 @@
       <c r="A22" s="6"/>
     </row>
     <row r="23" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="92" t="s">
         <v>143</v>
       </c>
       <c r="B23" s="59" t="s">
@@ -2871,31 +2914,31 @@
       </c>
     </row>
     <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="70"/>
+      <c r="A24" s="93"/>
       <c r="B24" s="59" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="70"/>
+      <c r="A25" s="93"/>
       <c r="B25" s="59" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="70"/>
+      <c r="A26" s="93"/>
       <c r="B26" s="59" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="70"/>
+      <c r="A27" s="93"/>
       <c r="B27" s="59" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="70"/>
+      <c r="A28" s="93"/>
       <c r="B28" s="59" t="s">
         <v>65</v>
       </c>
@@ -3371,6 +3414,17 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="24">
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="G9:H9"/>
@@ -3384,17 +3438,6 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="51" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -3405,7 +3448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68152F34-4C61-41C5-9C39-A3BBEA315BEB}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3414,7 +3457,7 @@
     <col min="1" max="1" width="54.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
         <v>112</v>
       </c>
@@ -3434,72 +3477,72 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="232" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="290" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="174" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="174" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="174" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>142</v>
       </c>
@@ -3511,168 +3554,174 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFD399D-BAFD-477C-886D-7EDCF3226FF1}">
-  <dimension ref="F6:K31"/>
+  <dimension ref="F6:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="16.36328125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" style="1" customWidth="1"/>
+    <col min="10" max="12" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F6" t="s">
+      <c r="F6" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="65" t="s">
         <v>155</v>
       </c>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
     </row>
     <row r="7" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F7" s="8">
+      <c r="F7" s="66">
         <v>45363</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H7" s="87">
+      <c r="H7" s="67">
         <v>-56485</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>-36556</v>
       </c>
     </row>
     <row r="8" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F8" s="8">
+      <c r="F8" s="66">
         <v>45363</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H8" s="87">
+      <c r="H8" s="67">
         <v>65213</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>65213</v>
       </c>
     </row>
     <row r="9" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F9" s="8">
+      <c r="F9" s="66">
         <v>45363</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H9" s="87">
+      <c r="H9" s="67">
         <v>-10000</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F10" s="8"/>
-      <c r="H10" s="87">
+      <c r="F10" s="66"/>
+      <c r="H10" s="67">
         <f>SUM(H7:H9)</f>
         <v>-1272</v>
       </c>
-      <c r="I10" s="87">
+      <c r="I10" s="67">
         <f>SUM(I7:I9)</f>
         <v>28657</v>
       </c>
-      <c r="J10" s="87">
+      <c r="J10" s="68">
         <f>I10-H10</f>
         <v>29929</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="69" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="11" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="J11" s="87"/>
+      <c r="J11" s="67"/>
     </row>
     <row r="12" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="J12" s="87"/>
+      <c r="J12" s="67"/>
     </row>
     <row r="13" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F13" s="8">
+      <c r="F13" s="66">
         <v>45601</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H13" s="87">
+      <c r="H13" s="67">
         <v>-76131</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>-88398</v>
       </c>
-      <c r="J13" s="87"/>
+      <c r="J13" s="67"/>
     </row>
     <row r="14" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F14" s="8">
+      <c r="F14" s="66">
         <v>45601</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H14" s="87">
+      <c r="H14" s="67">
         <v>95231</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>95231</v>
       </c>
-      <c r="J14" s="87"/>
+      <c r="J14" s="67"/>
     </row>
     <row r="15" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F15" s="8">
+      <c r="F15" s="66">
         <v>45601</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H15" s="87">
+      <c r="H15" s="67">
         <v>-3000</v>
       </c>
-      <c r="J15" s="87"/>
+      <c r="J15" s="67"/>
     </row>
     <row r="16" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="H16" s="87">
+      <c r="H16" s="67">
         <f>SUM(H13:H15)</f>
         <v>16100</v>
       </c>
-      <c r="I16" s="87">
+      <c r="I16" s="67">
         <f>SUM(I13:I15)</f>
         <v>6833</v>
       </c>
-      <c r="J16" s="87">
-        <f t="shared" ref="J11:J16" si="0">I16-H16</f>
+      <c r="J16" s="70">
+        <f t="shared" ref="J16" si="0">I16-H16</f>
         <v>-9267</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="71" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F22" s="87"/>
+      <c r="F22" s="67"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F25" s="87"/>
+      <c r="F25" s="67"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F28" s="87"/>
+      <c r="F28" s="67"/>
     </row>
     <row r="31" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F31" s="87"/>
+      <c r="F31" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3683,8 +3732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4000,18 +4049,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Kommentar0 xmlns="055c4a11-8173-45d4-8412-20d21b900f07" xsi:nil="true"/>
-    <Kategori xmlns="055c4a11-8173-45d4-8412-20d21b900f07">Teknisk dokumentation</Kategori>
-    <M_x00e5_lgrupp xmlns="055c4a11-8173-45d4-8412-20d21b900f07">
-      <Value>Konsumenter</Value>
-      <Value>IT-leverantörer</Value>
-    </M_x00e5_lgrupp>
-    <Kommentar xmlns="055c4a11-8173-45d4-8412-20d21b900f07">OK</Kommentar>
-    <Syfte xmlns="055c4a11-8173-45d4-8412-20d21b900f07" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4197,26 +4240,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Kommentar0 xmlns="055c4a11-8173-45d4-8412-20d21b900f07" xsi:nil="true"/>
+    <Kategori xmlns="055c4a11-8173-45d4-8412-20d21b900f07">Teknisk dokumentation</Kategori>
+    <M_x00e5_lgrupp xmlns="055c4a11-8173-45d4-8412-20d21b900f07">
+      <Value>Konsumenter</Value>
+      <Value>IT-leverantörer</Value>
+    </M_x00e5_lgrupp>
+    <Kommentar xmlns="055c4a11-8173-45d4-8412-20d21b900f07">OK</Kommentar>
+    <Syfte xmlns="055c4a11-8173-45d4-8412-20d21b900f07" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90CD9CF6-3488-4F16-8E76-7A648CC36ED2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{905DD5F0-F1C4-403B-AC12-3FD7F1CF9D2F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="055c4a11-8173-45d4-8412-20d21b900f07"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4240,9 +4281,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{905DD5F0-F1C4-403B-AC12-3FD7F1CF9D2F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90CD9CF6-3488-4F16-8E76-7A648CC36ED2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="055c4a11-8173-45d4-8412-20d21b900f07"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>